<commit_message>
add template match in opencv
</commit_message>
<xml_diff>
--- a/code/web/test/sample/pic.xlsx
+++ b/code/web/test/sample/pic.xlsx
@@ -16,48 +16,55 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
+    <t>195*280</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>198*283</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>220*220</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200*280</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>197*283</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>197*279</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99bfa9eff3fd1a75587bcee4e144061c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>426777d2191aa13ca816930a66157b8b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>4c475f9831414f259b51c36a53a89920</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a6b496de1c1329b670dd34386f96dbe3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>5a6f52f08bf901a6aed84778b36c4e9a</t>
-  </si>
-  <si>
-    <t>195*280</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>198*283</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>426777d2191aa13ca816930a66157b8b</t>
-  </si>
-  <si>
-    <t>a6b496de1c1329b670dd34386f96dbe3</t>
-  </si>
-  <si>
-    <t>220*220</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>99bfa9eff3fd1a75587bcee4e144061c</t>
-  </si>
-  <si>
-    <t>200*280</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>c75919625dcfdc5fd318d5da3532853c</t>
-  </si>
-  <si>
-    <t>197*283</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>e3c2c4b85ccd96d16eee6b5882d52b3d</t>
-  </si>
-  <si>
-    <t>197*279</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -681,7 +688,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -694,52 +701,52 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>3</v>
       </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>